<commit_message>
cambios viejos pre presentacion
</commit_message>
<xml_diff>
--- a/analisis/metologias/comparacion_estimaciones_renta_hidrocarburifera.xlsx
+++ b/analisis/metologias/comparacion_estimaciones_renta_hidrocarburifera.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Archivos\repos\pioYPFConicet\analisis\metologias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B01FE03-0C6D-45E9-8A02-7366A514403F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E561D608-FCBA-4A49-8793-6E5F2BDF9005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{A5002639-9EB3-4F56-8D1E-2FB527A288BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{A5002639-9EB3-4F56-8D1E-2FB527A288BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparacion estimaciones" sheetId="1" r:id="rId1"/>
@@ -267,9 +267,6 @@
     <t>(Producción - Exportaciones) * (Precio internacional * TCP - Precio venta interno * TCC)</t>
   </si>
   <si>
-    <t>(P * Q ) - CI - W - Gcia normal</t>
-  </si>
-  <si>
     <t>Gcia normal</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>UNCTAD / Informes de empresas</t>
+  </si>
+  <si>
+    <t>(P * Q * TCP ) - CI_ccnn - W_ccnn - Gcia normal</t>
   </si>
 </sst>
 </file>
@@ -868,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E47F69D-0C17-4BB1-AFE7-A8F9D60D3C0C}">
   <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="A33:C35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +899,7 @@
         <v>68</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1080,13 +1080,13 @@
         <v>24</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>30</v>
@@ -1117,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>32</v>
@@ -1134,7 +1134,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>32</v>
@@ -1219,7 +1219,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>1</v>
@@ -1434,7 +1434,7 @@
         <v>24</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1442,10 +1442,10 @@
         <v>74</v>
       </c>
       <c r="C35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46578C92-76E4-4EBB-ABD4-A406B03A2DD4}">
   <dimension ref="A2:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,13 +1477,13 @@
         <v>64</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,13 +1491,13 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
         <v>139</v>
-      </c>
-      <c r="D3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,13 +1505,13 @@
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,13 +1519,13 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,27 +1533,27 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1561,13 +1561,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,13 +1575,13 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" t="s">
         <v>132</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>133</v>
-      </c>
-      <c r="D9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1589,27 +1589,27 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,13 +1617,13 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
         <v>114</v>
       </c>
-      <c r="C12" t="s">
-        <v>115</v>
-      </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
         <v>126</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>127</v>
-      </c>
-      <c r="D13" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1645,27 +1645,27 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
         <v>116</v>
-      </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,13 +1673,13 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,13 +1687,13 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1701,27 +1701,27 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" t="s">
         <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
         <v>94</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,13 +1729,13 @@
         <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1743,13 +1743,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
         <v>122</v>
-      </c>
-      <c r="D21" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1757,13 +1757,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
         <v>130</v>
       </c>
-      <c r="C22" t="s">
-        <v>131</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,13 +1771,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1785,13 +1785,13 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,13 +1799,13 @@
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1813,13 +1813,13 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,27 +1841,27 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,13 +1869,13 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,13 +1883,13 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,27 +1897,27 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
         <v>90</v>
       </c>
-      <c r="C32" t="s">
-        <v>91</v>
-      </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>90</v>
       </c>
-      <c r="C33" t="s">
-        <v>91</v>
-      </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,27 +1925,27 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
         <v>90</v>
       </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,13 +1953,13 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,13 +1967,13 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,13 +1981,13 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1995,27 +1995,27 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s">
         <v>120</v>
       </c>
-      <c r="C39" t="s">
-        <v>121</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,13 +2023,13 @@
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2048,12 +2048,15 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="13" width="12.28515625" customWidth="1"/>
+    <col min="3" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="64.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>